<commit_message>
Correccion direcion IP Server0
</commit_message>
<xml_diff>
--- a/direcciones.xlsx
+++ b/direcciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhoen\OneDrive\Desktop\repos\omar-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\omar-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCA4499-7167-4283-BE88-E42D5672F08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FF4F11-4ABD-4C0C-B0D0-CA539BC9B2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1785" yWindow="1395" windowWidth="24375" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>Server0</t>
   </si>
   <si>
-    <t>10.1.1.5</t>
-  </si>
-  <si>
     <t>PC1</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>10.2.1.5</t>
   </si>
 </sst>
 </file>
@@ -491,10 +491,10 @@
   <dimension ref="B2:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -561,7 +561,7 @@
         <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" t="s">
@@ -583,7 +583,7 @@
         <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -629,13 +629,13 @@
         <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -651,16 +651,16 @@
         <v>255.255.255.0</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
         <v>38</v>
       </c>
-      <c r="M8" t="s">
-        <v>39</v>
-      </c>
       <c r="N8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -676,16 +676,16 @@
         <v>255.255.255.0</v>
       </c>
       <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" t="s">
         <v>37</v>
       </c>
-      <c r="L9" t="s">
-        <v>38</v>
-      </c>
       <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
         <v>40</v>
-      </c>
-      <c r="N9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>